<commit_message>
Run on 19-08-25. Also all date and time values are extracted from ist_date_get(). Also added one command to save analysed stock csv files onto disk. This is the most update file
</commit_message>
<xml_diff>
--- a/CURRENT STATUS/Current_status_2025-08-17.xlsx
+++ b/CURRENT STATUS/Current_status_2025-08-17.xlsx
@@ -506,10 +506,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C2" t="n">
-        <v>85.66</v>
+        <v>85.95</v>
       </c>
       <c r="D2" t="n">
         <v>25</v>
@@ -518,10 +518,10 @@
         <v>49</v>
       </c>
       <c r="F2" t="n">
-        <v>85.38300676805399</v>
+        <v>85.35992399872514</v>
       </c>
       <c r="G2" t="n">
-        <v>84.52603614344883</v>
+        <v>84.47878764942587</v>
       </c>
       <c r="H2" t="n">
         <v>14</v>
@@ -530,7 +530,7 @@
         <v>39</v>
       </c>
       <c r="J2" t="n">
-        <v>52.61357270293483</v>
+        <v>54.85323046071112</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C3" t="n">
-        <v>114.29</v>
+        <v>115.33</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -562,10 +562,10 @@
         <v>196</v>
       </c>
       <c r="F3" t="n">
-        <v>114.4909951330356</v>
+        <v>114.5484223139029</v>
       </c>
       <c r="G3" t="n">
-        <v>100.5843938452071</v>
+        <v>100.4438058193916</v>
       </c>
       <c r="H3" t="n">
         <v>5</v>
@@ -574,7 +574,7 @@
         <v>80</v>
       </c>
       <c r="J3" t="n">
-        <v>48.38490023243491</v>
+        <v>60.42799201266769</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -594,10 +594,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C4" t="n">
-        <v>48.89</v>
+        <v>48.23</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
@@ -606,10 +606,10 @@
         <v>48</v>
       </c>
       <c r="F4" t="n">
-        <v>48.6883570024921</v>
+        <v>48.64354744749035</v>
       </c>
       <c r="G4" t="n">
-        <v>49.43920296966345</v>
+        <v>49.46257330879806</v>
       </c>
       <c r="H4" t="n">
         <v>23</v>
@@ -618,7 +618,7 @@
         <v>47</v>
       </c>
       <c r="J4" t="n">
-        <v>46.31290612302494</v>
+        <v>41.54331864621257</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C5" t="n">
-        <v>266</v>
+        <v>263.12</v>
       </c>
       <c r="D5" t="n">
         <v>25</v>
@@ -650,10 +650,10 @@
         <v>45</v>
       </c>
       <c r="F5" t="n">
-        <v>264.2973675171605</v>
+        <v>264.1554814769239</v>
       </c>
       <c r="G5" t="n">
-        <v>264.3320281617751</v>
+        <v>264.2562112600376</v>
       </c>
       <c r="H5" t="n">
         <v>16</v>
@@ -662,7 +662,7 @@
         <v>62</v>
       </c>
       <c r="J5" t="n">
-        <v>54.09897664987549</v>
+        <v>46.2154049024081</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -682,10 +682,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C6" t="n">
-        <v>90.79000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -694,10 +694,10 @@
         <v>73</v>
       </c>
       <c r="F6" t="n">
-        <v>90.52074227386467</v>
+        <v>90.43098969848623</v>
       </c>
       <c r="G6" t="n">
-        <v>91.09516686163256</v>
+        <v>91.10364371890013</v>
       </c>
       <c r="H6" t="n">
         <v>17</v>
@@ -706,7 +706,7 @@
         <v>41</v>
       </c>
       <c r="J6" t="n">
-        <v>45.36133488044612</v>
+        <v>43.05394628655823</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -726,10 +726,10 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C7" t="n">
-        <v>169.94</v>
+        <v>168.06</v>
       </c>
       <c r="D7" t="n">
         <v>15</v>
@@ -738,10 +738,10 @@
         <v>35</v>
       </c>
       <c r="F7" t="n">
-        <v>170.4814546783116</v>
+        <v>170.5588053466418</v>
       </c>
       <c r="G7" t="n">
-        <v>172.283973531176</v>
+        <v>172.4218543271275</v>
       </c>
       <c r="H7" t="n">
         <v>30</v>
@@ -750,7 +750,7 @@
         <v>52</v>
       </c>
       <c r="J7" t="n">
-        <v>48.10954585844273</v>
+        <v>45.34208870124789</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -770,10 +770,10 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C8" t="n">
-        <v>21.97</v>
+        <v>21.69</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -782,10 +782,10 @@
         <v>60</v>
       </c>
       <c r="F8" t="n">
-        <v>21.78209558995996</v>
+        <v>21.71946078661329</v>
       </c>
       <c r="G8" t="n">
-        <v>21.87415662493617</v>
+        <v>21.8709076969679</v>
       </c>
       <c r="H8" t="n">
         <v>29</v>
@@ -794,7 +794,7 @@
         <v>46</v>
       </c>
       <c r="J8" t="n">
-        <v>50.90584281853676</v>
+        <v>47.40499544770443</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -814,10 +814,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C9" t="n">
-        <v>25.89</v>
+        <v>24.76</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
@@ -826,10 +826,10 @@
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>25.02804520711824</v>
+        <v>24.59706781067737</v>
       </c>
       <c r="G9" t="n">
-        <v>24.75964672104944</v>
+        <v>24.50845710350486</v>
       </c>
       <c r="H9" t="n">
         <v>13</v>
@@ -838,7 +838,7 @@
         <v>45</v>
       </c>
       <c r="J9" t="n">
-        <v>73.92351146742607</v>
+        <v>58.47951187331634</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C10" t="n">
-        <v>59.45</v>
+        <v>58.35</v>
       </c>
       <c r="D10" t="n">
         <v>12</v>
@@ -870,10 +870,10 @@
         <v>72</v>
       </c>
       <c r="F10" t="n">
-        <v>58.96439999951831</v>
+        <v>58.87610909033982</v>
       </c>
       <c r="G10" t="n">
-        <v>58.94671571099133</v>
+        <v>58.93253868876573</v>
       </c>
       <c r="H10" t="n">
         <v>29</v>
@@ -882,7 +882,7 @@
         <v>48</v>
       </c>
       <c r="J10" t="n">
-        <v>52.34714500744315</v>
+        <v>46.56604679968317</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -891,7 +891,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>B_N_Y</t>
+          <t>S</t>
         </is>
       </c>
     </row>
@@ -902,10 +902,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C11" t="n">
-        <v>149.69</v>
+        <v>150.22</v>
       </c>
       <c r="D11" t="n">
         <v>13</v>
@@ -914,10 +914,10 @@
         <v>106</v>
       </c>
       <c r="F11" t="n">
-        <v>148.7473199243045</v>
+        <v>148.5902065783553</v>
       </c>
       <c r="G11" t="n">
-        <v>145.5374766720767</v>
+        <v>145.4583809894505</v>
       </c>
       <c r="H11" t="n">
         <v>14</v>
@@ -926,7 +926,7 @@
         <v>45</v>
       </c>
       <c r="J11" t="n">
-        <v>53.35714677061585</v>
+        <v>55.12602049899276</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C12" t="n">
-        <v>205.79</v>
+        <v>204.89</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
@@ -958,10 +958,10 @@
         <v>164</v>
       </c>
       <c r="F12" t="n">
-        <v>204.369464607306</v>
+        <v>203.659196910959</v>
       </c>
       <c r="G12" t="n">
-        <v>186.417664959908</v>
+        <v>186.1799675974528</v>
       </c>
       <c r="H12" t="n">
         <v>30</v>
@@ -970,7 +970,7 @@
         <v>52</v>
       </c>
       <c r="J12" t="n">
-        <v>64.05320063555345</v>
+        <v>63.30069169431682</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -990,10 +990,10 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C13" t="n">
-        <v>376.73</v>
+        <v>379.83</v>
       </c>
       <c r="D13" t="n">
         <v>5</v>
@@ -1002,10 +1002,10 @@
         <v>83</v>
       </c>
       <c r="F13" t="n">
-        <v>377.9723110944171</v>
+        <v>378.5934666416255</v>
       </c>
       <c r="G13" t="n">
-        <v>401.255249349478</v>
+        <v>401.8534261628802</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
@@ -1014,7 +1014,7 @@
         <v>52</v>
       </c>
       <c r="J13" t="n">
-        <v>25.76066345775442</v>
+        <v>88.01200520444478</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1034,10 +1034,10 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C14" t="n">
-        <v>30.44</v>
+        <v>29.82</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1046,10 +1046,10 @@
         <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>29.84846277989558</v>
+        <v>29.67945214558003</v>
       </c>
       <c r="G14" t="n">
-        <v>29.83907765151208</v>
+        <v>29.81722592974812</v>
       </c>
       <c r="H14" t="n">
         <v>24</v>
@@ -1058,7 +1058,7 @@
         <v>44</v>
       </c>
       <c r="J14" t="n">
-        <v>54.45631618007259</v>
+        <v>49.1071985498797</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>B_N_Y</t>
+          <t>S</t>
         </is>
       </c>
     </row>
@@ -1078,10 +1078,10 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C15" t="n">
-        <v>571.6</v>
+        <v>567</v>
       </c>
       <c r="D15" t="n">
         <v>12</v>
@@ -1090,10 +1090,10 @@
         <v>42</v>
       </c>
       <c r="F15" t="n">
-        <v>568.8924992644634</v>
+        <v>568.4002264034567</v>
       </c>
       <c r="G15" t="n">
-        <v>571.4229692025443</v>
+        <v>571.4143335538879</v>
       </c>
       <c r="H15" t="n">
         <v>22</v>
@@ -1102,7 +1102,7 @@
         <v>43</v>
       </c>
       <c r="J15" t="n">
-        <v>50.23032669197816</v>
+        <v>46.26793764435742</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1122,10 +1122,10 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C16" t="n">
-        <v>3413.5</v>
+        <v>3265.4</v>
       </c>
       <c r="D16" t="n">
         <v>64</v>
@@ -1134,10 +1134,10 @@
         <v>180</v>
       </c>
       <c r="F16" t="n">
-        <v>3141.556134197419</v>
+        <v>3132.922995600512</v>
       </c>
       <c r="G16" t="n">
-        <v>2987.358948969164</v>
+        <v>2982.59759644368</v>
       </c>
       <c r="H16" t="n">
         <v>7</v>
@@ -1146,7 +1146,7 @@
         <v>18</v>
       </c>
       <c r="J16" t="n">
-        <v>78.42786843109567</v>
+        <v>61.67310218031128</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1166,10 +1166,10 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45887</v>
+        <v>45883</v>
       </c>
       <c r="C17" t="n">
-        <v>2010.6</v>
+        <v>1936.6</v>
       </c>
       <c r="D17" t="n">
         <v>22</v>
@@ -1178,10 +1178,10 @@
         <v>105</v>
       </c>
       <c r="F17" t="n">
-        <v>2097.239022376044</v>
+        <v>2105.49035784043</v>
       </c>
       <c r="G17" t="n">
-        <v>2232.317549355533</v>
+        <v>2236.581348381601</v>
       </c>
       <c r="H17" t="n">
         <v>5</v>
@@ -1190,7 +1190,7 @@
         <v>39</v>
       </c>
       <c r="J17" t="n">
-        <v>50.61794105653752</v>
+        <v>22.05728328164675</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>

</xml_diff>